<commit_message>
updated styles and calculation engine
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajikumarjs/personal/reli_engine/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2B9F07-B6FC-424B-8EC2-76F744A1B594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED654546-E182-0D4E-8467-AB2BD585AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" activeTab="1" xr2:uid="{C431CB80-CA07-A34D-829D-C72251BD8198}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" activeTab="1" xr2:uid="{C431CB80-CA07-A34D-829D-C72251BD8198}"/>
   </bookViews>
   <sheets>
     <sheet name="component" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="100">
   <si>
     <t>carbon film</t>
   </si>
@@ -255,15 +255,6 @@
     <t>Inductors</t>
   </si>
   <si>
-    <t>U/Umax ≤ 0.1, Uref/Umax 0.5</t>
-  </si>
-  <si>
-    <t>U/Umax 0.7, Uref/Umax 0.5</t>
-  </si>
-  <si>
-    <t>U/Umax 1, Uref/Umax 0.5</t>
-  </si>
-  <si>
     <t>Degree of Integration LSI &gt; 100, &gt; 500</t>
   </si>
   <si>
@@ -310,9 +301,6 @@
   </si>
   <si>
     <t>101 - 125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switches and buttons for higher electrical load </t>
   </si>
   <si>
     <r>
@@ -344,7 +332,28 @@
     <t>Voltage  ratio U/Umax</t>
   </si>
   <si>
-    <t xml:space="preserve">Switches and buttons for light-current applications </t>
+    <t>Z-Diodes</t>
+  </si>
+  <si>
+    <t>Uref/Umax 0.5</t>
+  </si>
+  <si>
+    <t>U/Umax</t>
+  </si>
+  <si>
+    <t>light-current applications</t>
+  </si>
+  <si>
+    <t>Switches and buttons</t>
+  </si>
+  <si>
+    <t>higher electrical load</t>
+  </si>
+  <si>
+    <t>&lt;=0.1</t>
+  </si>
+  <si>
+    <t>"Digital logic families and bus interfaces,busdriver and receiver circuit"</t>
   </si>
 </sst>
 </file>
@@ -789,7 +798,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,7 +1181,7 @@
         <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E19" s="1">
         <v>5</v>
@@ -1226,7 +1235,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>63</v>
@@ -1292,7 +1301,7 @@
         <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="E25" s="1">
         <v>0.7</v>
@@ -1312,7 +1321,7 @@
         <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1332,7 +1341,7 @@
         <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1349,7 +1358,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1369,7 +1378,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1389,7 +1398,7 @@
         <v>71</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1406,7 +1415,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -1423,13 +1432,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E32" s="1">
         <v>0.5</v>
@@ -1440,13 +1449,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
         <v>81</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" t="s">
-        <v>84</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -1457,10 +1466,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -1474,7 +1483,7 @@
         <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="E35" s="1">
         <v>2</v>
@@ -1485,10 +1494,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -1556,11 +1565,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D113D345-D12B-094C-864F-935BFCFCA585}">
-  <dimension ref="A1:R167"/>
+  <dimension ref="A1:Q173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O162" sqref="O162"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P143" sqref="P143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1568,11 +1577,12 @@
     <col min="2" max="2" width="57.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="10.83203125" style="1"/>
     <col min="14" max="14" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1618,8 +1628,11 @@
       <c r="O1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1653,7 +1666,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1670,7 +1683,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1687,7 +1700,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1721,7 +1734,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1738,7 +1751,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1755,7 +1768,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1772,7 +1785,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1789,7 +1802,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1806,7 +1819,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1823,7 +1836,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1840,7 +1853,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1857,7 +1870,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3439,7 +3452,7 @@
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
       <c r="N105" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O105" s="1" t="s">
         <v>55</v>
@@ -3474,7 +3487,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
       <c r="N106" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O106" s="1" t="s">
         <v>55</v>
@@ -3509,7 +3522,7 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
       <c r="N107" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>55</v>
@@ -3544,7 +3557,7 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
       <c r="N108" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O108" s="1">
         <v>1</v>
@@ -3579,7 +3592,7 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
       <c r="N109" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O109" s="1">
         <v>1</v>
@@ -3614,7 +3627,7 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
       <c r="N110" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="O110" s="1">
         <v>1</v>
@@ -3625,7 +3638,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C111" s="1">
         <v>45</v>
@@ -3649,7 +3662,7 @@
       <c r="N111" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O111" s="1" t="s">
+      <c r="O111" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3658,7 +3671,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C112" s="1">
         <v>45</v>
@@ -3682,7 +3695,7 @@
       <c r="N112" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O112" s="1" t="s">
+      <c r="O112" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3691,7 +3704,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C113" s="1">
         <v>45</v>
@@ -3715,7 +3728,7 @@
       <c r="N113" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O113" s="1" t="s">
+      <c r="O113" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3724,7 +3737,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C114" s="1">
         <v>45</v>
@@ -3757,7 +3770,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C115" s="1">
         <v>45</v>
@@ -3790,7 +3803,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C116" s="1">
         <v>45</v>
@@ -3847,9 +3860,9 @@
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
       <c r="N117" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O117" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O117" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3882,9 +3895,9 @@
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
       <c r="N118" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O118" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O118" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3917,9 +3930,9 @@
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
       <c r="N119" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O119" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O119" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3952,7 +3965,7 @@
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
       <c r="N120" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O120" s="1">
         <v>0.5</v>
@@ -3987,7 +4000,7 @@
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
       <c r="N121" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O121" s="1">
         <v>0.5</v>
@@ -4022,7 +4035,7 @@
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
       <c r="N122" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O122" s="1">
         <v>0.5</v>
@@ -4057,7 +4070,7 @@
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
       <c r="N123" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O123" s="1">
         <v>1</v>
@@ -4092,7 +4105,7 @@
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O124" s="1">
         <v>1</v>
@@ -4127,7 +4140,7 @@
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="O125" s="1">
         <v>1</v>
@@ -4205,7 +4218,7 @@
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4229,7 +4242,7 @@
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4253,7 +4266,7 @@
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4277,7 +4290,7 @@
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4301,7 +4314,7 @@
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4325,7 +4338,7 @@
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4349,7 +4362,7 @@
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4378,13 +4391,16 @@
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
       <c r="N135" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="O135" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P135" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4413,13 +4429,16 @@
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
       <c r="N136" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O136" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O136" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P136" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4448,13 +4467,16 @@
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
       <c r="N137" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O137" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O137" s="1">
+        <v>1</v>
+      </c>
+      <c r="P137" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4483,13 +4505,16 @@
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
       <c r="N138" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="O138" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P138" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4518,13 +4543,16 @@
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
       <c r="N139" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O139" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O139" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P139" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4553,13 +4581,16 @@
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
       <c r="N140" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O140" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O140" s="1">
+        <v>1</v>
+      </c>
+      <c r="P140" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4588,13 +4619,16 @@
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
       <c r="N141" s="1" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="O141" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P141" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4623,13 +4657,16 @@
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
       <c r="N142" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O142" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O142" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P142" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4658,13 +4695,16 @@
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
       <c r="N143" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O143" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O143" s="1">
+        <v>1</v>
+      </c>
+      <c r="P143" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4675,7 +4715,7 @@
         <v>60</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E144" s="1">
         <v>0.75</v>
@@ -4688,7 +4728,7 @@
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4712,7 +4752,7 @@
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4736,7 +4776,7 @@
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4747,7 +4787,7 @@
         <v>85</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E147" s="1">
         <v>0.43</v>
@@ -4760,7 +4800,7 @@
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4784,7 +4824,7 @@
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4808,7 +4848,7 @@
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4819,7 +4859,7 @@
         <v>55</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E150" s="1">
         <v>0.79</v>
@@ -4832,7 +4872,7 @@
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4856,7 +4896,7 @@
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4880,12 +4920,12 @@
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
@@ -4895,12 +4935,12 @@
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E154" s="1">
         <v>1</v>
@@ -4919,18 +4959,18 @@
       </c>
       <c r="M154" s="1"/>
       <c r="N154" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E155" s="1">
         <v>1.8</v>
@@ -4949,18 +4989,18 @@
       </c>
       <c r="M155" s="1"/>
       <c r="N155" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E156" s="1">
         <v>4</v>
@@ -4979,18 +5019,18 @@
       </c>
       <c r="M156" s="1"/>
       <c r="N156" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O156" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O156" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E157" s="1">
         <v>1</v>
@@ -5009,18 +5049,18 @@
       </c>
       <c r="M157" s="1"/>
       <c r="N157" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E158" s="1">
         <v>1.8</v>
@@ -5039,18 +5079,18 @@
       </c>
       <c r="M158" s="1"/>
       <c r="N158" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E159" s="1">
         <v>4</v>
@@ -5069,13 +5109,13 @@
       </c>
       <c r="M159" s="1"/>
       <c r="N159" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O159" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O159" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5093,19 +5133,16 @@
       </c>
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
-      <c r="N160" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P160" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
@@ -5118,14 +5155,11 @@
       </c>
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
-      <c r="N161" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O161" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P161" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5139,10 +5173,10 @@
         <v>58</v>
       </c>
       <c r="O162" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5159,7 +5193,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5176,7 +5210,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5196,13 +5230,13 @@
         <v>0.15</v>
       </c>
       <c r="N165" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="O165" s="1">
         <v>0.33</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5222,13 +5256,13 @@
         <v>1</v>
       </c>
       <c r="N166" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="O166" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5248,11 +5282,155 @@
         <v>15</v>
       </c>
       <c r="N167" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="O167" s="1">
         <v>4</v>
       </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>92</v>
+      </c>
+      <c r="C168" s="1">
+        <v>55</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E168" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>92</v>
+      </c>
+      <c r="C169" s="1">
+        <v>55</v>
+      </c>
+      <c r="D169" s="1">
+        <v>60</v>
+      </c>
+      <c r="E169" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>92</v>
+      </c>
+      <c r="C170" s="1">
+        <v>55</v>
+      </c>
+      <c r="D170" s="1">
+        <v>200</v>
+      </c>
+      <c r="E170" s="1">
+        <v>77</v>
+      </c>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+    </row>
+    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>92</v>
+      </c>
+      <c r="C171" s="1">
+        <v>40</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E171" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="M171" s="1"/>
+    </row>
+    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>92</v>
+      </c>
+      <c r="C172" s="1">
+        <v>40</v>
+      </c>
+      <c r="D172" s="1">
+        <v>60</v>
+      </c>
+      <c r="E172" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="1"/>
+    </row>
+    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>92</v>
+      </c>
+      <c r="C173" s="1">
+        <v>40</v>
+      </c>
+      <c r="D173" s="1">
+        <v>200</v>
+      </c>
+      <c r="E173" s="1">
+        <v>151</v>
+      </c>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>